<commit_message>
permak dikit excel main_owner.py
</commit_message>
<xml_diff>
--- a/datapenjualan_platinum.xlsx
+++ b/datapenjualan_platinum.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,8 @@
     <col width="15.6" customWidth="1" min="6" max="6"/>
     <col width="7.199999999999999" customWidth="1" min="7" max="7"/>
     <col width="15.6" customWidth="1" min="8" max="8"/>
-    <col width="16.8" customWidth="1" min="9" max="9"/>
+    <col width="14.4" customWidth="1" min="9" max="9"/>
+    <col width="10.8" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -497,7 +498,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>LAPORAN PENJUALAN PER TANGGAL 01-06-2025 s/d 30-06-2025</t>
+          <t>LAPORAN PENJUALAN PERIODE 01-06-2025 s/d 30-06-2025</t>
         </is>
       </c>
       <c r="B2" s="4" t="n"/>
@@ -553,7 +554,12 @@
       </c>
       <c r="I4" s="5" t="inlineStr">
         <is>
-          <t>Metode bayar</t>
+          <t>Pembulatan</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>Bayar</t>
         </is>
       </c>
     </row>
@@ -595,10 +601,11 @@
       <c r="H5" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I5" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="6">
@@ -639,10 +646,11 @@
       <c r="H6" s="8" t="n">
         <v>700000</v>
       </c>
-      <c r="I6" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8" t="n">
+        <v>700000</v>
       </c>
     </row>
     <row r="7">
@@ -683,10 +691,11 @@
       <c r="H7" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I7" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="8">
@@ -727,10 +736,11 @@
       <c r="H8" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I8" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="9">
@@ -771,10 +781,11 @@
       <c r="H9" s="8" t="n">
         <v>630000</v>
       </c>
-      <c r="I9" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>630000</v>
       </c>
     </row>
     <row r="10">
@@ -815,10 +826,11 @@
       <c r="H10" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I10" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="11">
@@ -859,10 +871,11 @@
       <c r="H11" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I11" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="12">
@@ -903,10 +916,11 @@
       <c r="H12" s="8" t="n">
         <v>630000</v>
       </c>
-      <c r="I12" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8" t="n">
+        <v>630000</v>
       </c>
     </row>
     <row r="13">
@@ -947,10 +961,11 @@
       <c r="H13" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I13" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="14">
@@ -991,10 +1006,11 @@
       <c r="H14" s="8" t="n">
         <v>700000</v>
       </c>
-      <c r="I14" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8" t="n">
+        <v>700000</v>
       </c>
     </row>
     <row r="15">
@@ -1035,10 +1051,11 @@
       <c r="H15" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I15" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I15" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="16">
@@ -1079,10 +1096,11 @@
       <c r="H16" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I16" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="17">
@@ -1123,10 +1141,11 @@
       <c r="H17" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I17" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="18">
@@ -1167,10 +1186,11 @@
       <c r="H18" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I18" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="19">
@@ -1211,10 +1231,11 @@
       <c r="H19" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I19" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="20">
@@ -1255,10 +1276,11 @@
       <c r="H20" s="8" t="n">
         <v>200000</v>
       </c>
-      <c r="I20" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8" t="n">
+        <v>200000</v>
       </c>
     </row>
     <row r="21">
@@ -1299,10 +1321,11 @@
       <c r="H21" s="8" t="n">
         <v>6187500</v>
       </c>
-      <c r="I21" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I21" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8" t="n">
+        <v>6187500</v>
       </c>
     </row>
     <row r="22">
@@ -1343,10 +1366,11 @@
       <c r="H22" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I22" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I22" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="23">
@@ -1387,10 +1411,11 @@
       <c r="H23" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I23" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="24">
@@ -1431,10 +1456,11 @@
       <c r="H24" s="8" t="n">
         <v>700000</v>
       </c>
-      <c r="I24" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="8" t="n">
+        <v>700000</v>
       </c>
     </row>
     <row r="25">
@@ -1475,10 +1501,11 @@
       <c r="H25" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I25" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="26">
@@ -1519,10 +1546,11 @@
       <c r="H26" s="8" t="n">
         <v>800000</v>
       </c>
-      <c r="I26" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I26" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="8" t="n">
+        <v>800000</v>
       </c>
     </row>
     <row r="27">
@@ -1563,10 +1591,11 @@
       <c r="H27" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I27" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I27" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="28">
@@ -1607,10 +1636,11 @@
       <c r="H28" s="8" t="n">
         <v>750000</v>
       </c>
-      <c r="I28" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I28" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="8" t="n">
+        <v>750000</v>
       </c>
     </row>
     <row r="29">
@@ -1651,10 +1681,11 @@
       <c r="H29" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I29" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I29" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="30">
@@ -1695,10 +1726,11 @@
       <c r="H30" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I30" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I30" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="31">
@@ -1739,10 +1771,11 @@
       <c r="H31" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I31" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I31" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="32">
@@ -1783,10 +1816,11 @@
       <c r="H32" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I32" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I32" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="33">
@@ -1827,10 +1861,11 @@
       <c r="H33" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I33" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I33" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="34">
@@ -1871,10 +1906,11 @@
       <c r="H34" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I34" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I34" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="35">
@@ -1915,10 +1951,11 @@
       <c r="H35" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I35" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I35" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="36">
@@ -1959,10 +1996,11 @@
       <c r="H36" s="8" t="n">
         <v>800000</v>
       </c>
-      <c r="I36" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I36" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="8" t="n">
+        <v>800000</v>
       </c>
     </row>
     <row r="37">
@@ -2003,10 +2041,11 @@
       <c r="H37" s="8" t="n">
         <v>800000</v>
       </c>
-      <c r="I37" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I37" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="8" t="n">
+        <v>800000</v>
       </c>
     </row>
     <row r="38">
@@ -2047,10 +2086,11 @@
       <c r="H38" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I38" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I38" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="39">
@@ -2091,10 +2131,11 @@
       <c r="H39" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I39" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I39" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="40">
@@ -2135,10 +2176,11 @@
       <c r="H40" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I40" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I40" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="41">
@@ -2179,10 +2221,11 @@
       <c r="H41" s="8" t="n">
         <v>742500</v>
       </c>
-      <c r="I41" s="6" t="inlineStr">
-        <is>
-          <t>kredit</t>
-        </is>
+      <c r="I41" s="8" t="n">
+        <v>500</v>
+      </c>
+      <c r="J41" s="8" t="n">
+        <v>743000</v>
       </c>
     </row>
     <row r="42">
@@ -2223,10 +2266,11 @@
       <c r="H42" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I42" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I42" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="43">
@@ -2267,10 +2311,11 @@
       <c r="H43" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I43" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I43" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="44">
@@ -2311,10 +2356,11 @@
       <c r="H44" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I44" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I44" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="45">
@@ -2355,10 +2401,11 @@
       <c r="H45" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I45" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I45" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="46">
@@ -2399,10 +2446,11 @@
       <c r="H46" s="8" t="n">
         <v>700000</v>
       </c>
-      <c r="I46" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I46" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="8" t="n">
+        <v>700000</v>
       </c>
     </row>
     <row r="47">
@@ -2443,10 +2491,11 @@
       <c r="H47" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I47" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I47" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="48">
@@ -2487,10 +2536,11 @@
       <c r="H48" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I48" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I48" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="49">
@@ -2531,10 +2581,11 @@
       <c r="H49" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I49" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I49" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="50">
@@ -2575,10 +2626,11 @@
       <c r="H50" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I50" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I50" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="51">
@@ -2619,10 +2671,11 @@
       <c r="H51" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I51" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I51" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="52">
@@ -2663,10 +2716,11 @@
       <c r="H52" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I52" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I52" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="53">
@@ -2707,10 +2761,11 @@
       <c r="H53" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I53" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I53" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="54">
@@ -2751,10 +2806,11 @@
       <c r="H54" s="8" t="n">
         <v>630000</v>
       </c>
-      <c r="I54" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I54" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="8" t="n">
+        <v>630000</v>
       </c>
     </row>
     <row r="55">
@@ -2795,10 +2851,11 @@
       <c r="H55" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I55" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I55" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="56">
@@ -2839,10 +2896,11 @@
       <c r="H56" s="8" t="n">
         <v>35000</v>
       </c>
-      <c r="I56" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I56" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="8" t="n">
+        <v>35000</v>
       </c>
     </row>
     <row r="57">
@@ -2883,10 +2941,11 @@
       <c r="H57" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I57" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I57" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="58">
@@ -2927,10 +2986,11 @@
       <c r="H58" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I58" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I58" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="59">
@@ -2971,10 +3031,11 @@
       <c r="H59" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I59" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I59" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="60">
@@ -3015,10 +3076,11 @@
       <c r="H60" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I60" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I60" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="61">
@@ -3059,10 +3121,11 @@
       <c r="H61" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I61" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I61" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="62">
@@ -3103,10 +3166,11 @@
       <c r="H62" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I62" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I62" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="63">
@@ -3147,10 +3211,11 @@
       <c r="H63" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I63" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I63" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="64">
@@ -3191,10 +3256,11 @@
       <c r="H64" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I64" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I64" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="65">
@@ -3235,10 +3301,11 @@
       <c r="H65" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I65" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I65" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="66">
@@ -3279,10 +3346,11 @@
       <c r="H66" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I66" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I66" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="67">
@@ -3323,10 +3391,11 @@
       <c r="H67" s="8" t="n">
         <v>495000</v>
       </c>
-      <c r="I67" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I67" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" s="8" t="n">
+        <v>495000</v>
       </c>
     </row>
     <row r="68">
@@ -3367,10 +3436,11 @@
       <c r="H68" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I68" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I68" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="69">
@@ -3411,10 +3481,11 @@
       <c r="H69" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I69" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I69" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="70">
@@ -3455,10 +3526,11 @@
       <c r="H70" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I70" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I70" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="71">
@@ -3499,10 +3571,11 @@
       <c r="H71" s="8" t="n">
         <v>200000</v>
       </c>
-      <c r="I71" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I71" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" s="8" t="n">
+        <v>200000</v>
       </c>
     </row>
     <row r="72">
@@ -3543,10 +3616,11 @@
       <c r="H72" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I72" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I72" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="73">
@@ -3587,10 +3661,11 @@
       <c r="H73" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I73" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I73" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="74">
@@ -3631,10 +3706,11 @@
       <c r="H74" s="8" t="n">
         <v>550000</v>
       </c>
-      <c r="I74" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I74" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" s="8" t="n">
+        <v>550000</v>
       </c>
     </row>
     <row r="75">
@@ -3675,10 +3751,11 @@
       <c r="H75" s="8" t="n">
         <v>700000</v>
       </c>
-      <c r="I75" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I75" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" s="8" t="n">
+        <v>700000</v>
       </c>
     </row>
     <row r="76">
@@ -3719,10 +3796,11 @@
       <c r="H76" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I76" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I76" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="77">
@@ -3763,10 +3841,11 @@
       <c r="H77" s="8" t="n">
         <v>700000</v>
       </c>
-      <c r="I77" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I77" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" s="8" t="n">
+        <v>700000</v>
       </c>
     </row>
     <row r="78">
@@ -3807,10 +3886,11 @@
       <c r="H78" s="8" t="n">
         <v>742500</v>
       </c>
-      <c r="I78" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I78" s="8" t="n">
+        <v>500</v>
+      </c>
+      <c r="J78" s="8" t="n">
+        <v>743000</v>
       </c>
     </row>
     <row r="79">
@@ -3851,10 +3931,11 @@
       <c r="H79" s="8" t="n">
         <v>1800000</v>
       </c>
-      <c r="I79" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I79" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="8" t="n">
+        <v>1800000</v>
       </c>
     </row>
     <row r="80">
@@ -3895,10 +3976,11 @@
       <c r="H80" s="8" t="n">
         <v>800000</v>
       </c>
-      <c r="I80" s="6" t="inlineStr">
-        <is>
-          <t>qris</t>
-        </is>
+      <c r="I80" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="8" t="n">
+        <v>800000</v>
       </c>
     </row>
     <row r="81">
@@ -3939,10 +4021,11 @@
       <c r="H81" s="8" t="n">
         <v>50000</v>
       </c>
-      <c r="I81" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I81" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" s="8" t="n">
+        <v>50000</v>
       </c>
     </row>
     <row r="82">
@@ -3983,10 +4066,11 @@
       <c r="H82" s="8" t="n">
         <v>60000</v>
       </c>
-      <c r="I82" s="6" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
+      <c r="I82" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="8" t="n">
+        <v>60000</v>
       </c>
     </row>
     <row r="83">
@@ -4027,10 +4111,11 @@
       <c r="H83" s="8" t="n">
         <v>585000</v>
       </c>
-      <c r="I83" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I83" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="8" t="n">
+        <v>585000</v>
       </c>
     </row>
     <row r="84">
@@ -4071,10 +4156,11 @@
       <c r="H84" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I84" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I84" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="85">
@@ -4115,10 +4201,11 @@
       <c r="H85" s="8" t="n">
         <v>650000</v>
       </c>
-      <c r="I85" s="6" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
+      <c r="I85" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="8" t="n">
+        <v>650000</v>
       </c>
     </row>
     <row r="87">
@@ -4134,8 +4221,9 @@
       <c r="F87" s="9" t="inlineStr"/>
       <c r="G87" s="9" t="inlineStr"/>
       <c r="H87" s="9" t="inlineStr"/>
-      <c r="I87" s="10" t="n">
-        <v>52432500</v>
+      <c r="I87" s="9" t="inlineStr"/>
+      <c r="J87" s="10" t="n">
+        <v>52433500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save localku yg terakhir
</commit_message>
<xml_diff>
--- a/datapenjualan_platinum.xlsx
+++ b/datapenjualan_platinum.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,13 +1061,13 @@
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
-          <t>TF0014</t>
+          <t>TF0015</t>
         </is>
       </c>
       <c r="B16" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-18:45:56</t>
+18:47:39</t>
         </is>
       </c>
       <c r="C16" s="6" t="inlineStr">
@@ -1077,12 +1077,12 @@
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>04</t>
         </is>
       </c>
       <c r="E16" s="6" t="inlineStr">
         <is>
-          <t>Sherly</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F16" s="8" t="n">
@@ -1090,29 +1090,29 @@
       </c>
       <c r="G16" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H16" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
       <c r="I16" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>TF0015</t>
+          <t>TF0016</t>
         </is>
       </c>
       <c r="B17" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-18:47:39</t>
+18:57:00</t>
         </is>
       </c>
       <c r="C17" s="6" t="inlineStr">
@@ -1122,12 +1122,12 @@
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E17" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Sherly</t>
         </is>
       </c>
       <c r="F17" s="8" t="n">
@@ -1151,77 +1151,77 @@
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>TF0016</t>
+          <t>TF0018</t>
         </is>
       </c>
       <c r="B18" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-18:57:00</t>
+19:39:57</t>
         </is>
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>Fasilitas</t>
         </is>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E18" s="6" t="inlineStr">
         <is>
-          <t>Sherly</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F18" s="8" t="n">
-        <v>550000</v>
+        <v>200000</v>
       </c>
       <c r="G18" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H18" s="8" t="n">
-        <v>495000</v>
+        <v>200000</v>
       </c>
       <c r="I18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J18" s="8" t="n">
-        <v>495000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
         <is>
-          <t>TF0017</t>
+          <t>TF0019</t>
         </is>
       </c>
       <c r="B19" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-19:37:44</t>
+19:43:06</t>
         </is>
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>member</t>
         </is>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E19" s="6" t="inlineStr">
         <is>
-          <t>andin</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F19" s="8" t="n">
-        <v>650000</v>
+        <v>6187500</v>
       </c>
       <c r="G19" s="6" t="inlineStr">
         <is>
@@ -1229,44 +1229,44 @@
         </is>
       </c>
       <c r="H19" s="8" t="n">
-        <v>650000</v>
+        <v>6187500</v>
       </c>
       <c r="I19" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J19" s="8" t="n">
-        <v>650000</v>
+        <v>6187500</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
-          <t>TF0018</t>
+          <t>TF0054</t>
         </is>
       </c>
       <c r="B20" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-19:39:57</t>
+20:42:37</t>
         </is>
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>Fasilitas</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="D20" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E20" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>andin</t>
         </is>
       </c>
       <c r="F20" s="8" t="n">
-        <v>200000</v>
+        <v>550000</v>
       </c>
       <c r="G20" s="6" t="inlineStr">
         <is>
@@ -1274,44 +1274,44 @@
         </is>
       </c>
       <c r="H20" s="8" t="n">
-        <v>200000</v>
+        <v>550000</v>
       </c>
       <c r="I20" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="8" t="n">
-        <v>200000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
         <is>
-          <t>TF0019</t>
+          <t>TF0056</t>
         </is>
       </c>
       <c r="B21" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-19:43:06</t>
+20:44:52</t>
         </is>
       </c>
       <c r="C21" s="6" t="inlineStr">
         <is>
-          <t>member</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E21" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Qila</t>
         </is>
       </c>
       <c r="F21" s="8" t="n">
-        <v>6187500</v>
+        <v>550000</v>
       </c>
       <c r="G21" s="6" t="inlineStr">
         <is>
@@ -1319,25 +1319,25 @@
         </is>
       </c>
       <c r="H21" s="8" t="n">
-        <v>6187500</v>
+        <v>550000</v>
       </c>
       <c r="I21" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="8" t="n">
-        <v>6187500</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>TF0054</t>
+          <t>TF0057</t>
         </is>
       </c>
       <c r="B22" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-20:42:37</t>
+20:58:21</t>
         </is>
       </c>
       <c r="C22" s="6" t="inlineStr">
@@ -1347,16 +1347,16 @@
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>08</t>
         </is>
       </c>
       <c r="E22" s="6" t="inlineStr">
         <is>
-          <t>andin</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F22" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
       <c r="G22" s="6" t="inlineStr">
         <is>
@@ -1364,25 +1364,25 @@
         </is>
       </c>
       <c r="H22" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
       <c r="I22" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>TF0056</t>
+          <t>TF0058</t>
         </is>
       </c>
       <c r="B23" s="7" t="inlineStr">
         <is>
           <t>20-06-2025
-20:44:52</t>
+21:20:28</t>
         </is>
       </c>
       <c r="C23" s="6" t="inlineStr">
@@ -1392,12 +1392,12 @@
       </c>
       <c r="D23" s="6" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>09</t>
         </is>
       </c>
       <c r="E23" s="6" t="inlineStr">
         <is>
-          <t>Qila</t>
+          <t>Febby</t>
         </is>
       </c>
       <c r="F23" s="8" t="n">
@@ -1405,29 +1405,29 @@
       </c>
       <c r="G23" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H23" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
       <c r="I23" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>TF0057</t>
+          <t>TF0060</t>
         </is>
       </c>
       <c r="B24" s="7" t="inlineStr">
         <is>
-          <t>20-06-2025
-20:58:21</t>
+          <t>21-06-2025
+11:03:22</t>
         </is>
       </c>
       <c r="C24" s="6" t="inlineStr">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>01</t>
         </is>
       </c>
       <c r="E24" s="6" t="inlineStr">
@@ -1446,7 +1446,7 @@
         </is>
       </c>
       <c r="F24" s="8" t="n">
-        <v>700000</v>
+        <v>800000</v>
       </c>
       <c r="G24" s="6" t="inlineStr">
         <is>
@@ -1454,25 +1454,25 @@
         </is>
       </c>
       <c r="H24" s="8" t="n">
-        <v>700000</v>
+        <v>800000</v>
       </c>
       <c r="I24" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="8" t="n">
-        <v>700000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
         <is>
-          <t>TF0058</t>
+          <t>TF0061</t>
         </is>
       </c>
       <c r="B25" s="7" t="inlineStr">
         <is>
-          <t>20-06-2025
-21:20:28</t>
+          <t>21-06-2025
+12:17:08</t>
         </is>
       </c>
       <c r="C25" s="6" t="inlineStr">
@@ -1482,42 +1482,42 @@
       </c>
       <c r="D25" s="6" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>02</t>
         </is>
       </c>
       <c r="E25" s="6" t="inlineStr">
         <is>
-          <t>Febby</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F25" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="G25" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H25" s="8" t="n">
-        <v>495000</v>
+        <v>650000</v>
       </c>
       <c r="I25" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="8" t="n">
-        <v>495000</v>
+        <v>650000</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
         <is>
-          <t>TF0060</t>
+          <t>TF0062</t>
         </is>
       </c>
       <c r="B26" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-11:03:22</t>
+12:58:32</t>
         </is>
       </c>
       <c r="C26" s="6" t="inlineStr">
@@ -1527,16 +1527,16 @@
       </c>
       <c r="D26" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E26" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Qila</t>
         </is>
       </c>
       <c r="F26" s="8" t="n">
-        <v>800000</v>
+        <v>550000</v>
       </c>
       <c r="G26" s="6" t="inlineStr">
         <is>
@@ -1544,25 +1544,25 @@
         </is>
       </c>
       <c r="H26" s="8" t="n">
-        <v>800000</v>
+        <v>750000</v>
       </c>
       <c r="I26" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="8" t="n">
-        <v>800000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>TF0061</t>
+          <t>TF0063</t>
         </is>
       </c>
       <c r="B27" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-12:17:08</t>
+13:46:56</t>
         </is>
       </c>
       <c r="C27" s="6" t="inlineStr">
@@ -1572,16 +1572,16 @@
       </c>
       <c r="D27" s="6" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="E27" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Nadia</t>
         </is>
       </c>
       <c r="F27" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="G27" s="6" t="inlineStr">
         <is>
@@ -1589,25 +1589,25 @@
         </is>
       </c>
       <c r="H27" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="I27" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
         <is>
-          <t>TF0062</t>
+          <t>TF0064</t>
         </is>
       </c>
       <c r="B28" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-12:58:32</t>
+13:47:52</t>
         </is>
       </c>
       <c r="C28" s="6" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>05</t>
         </is>
       </c>
       <c r="E28" s="6" t="inlineStr">
         <is>
-          <t>Qila</t>
+          <t>Dian</t>
         </is>
       </c>
       <c r="F28" s="8" t="n">
@@ -1634,25 +1634,25 @@
         </is>
       </c>
       <c r="H28" s="8" t="n">
-        <v>750000</v>
+        <v>550000</v>
       </c>
       <c r="I28" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J28" s="8" t="n">
-        <v>750000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
         <is>
-          <t>TF0063</t>
+          <t>TF0065</t>
         </is>
       </c>
       <c r="B29" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-13:46:56</t>
+14:38:42</t>
         </is>
       </c>
       <c r="C29" s="6" t="inlineStr">
@@ -1662,16 +1662,16 @@
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E29" s="6" t="inlineStr">
         <is>
-          <t>Nadia</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F29" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="G29" s="6" t="inlineStr">
         <is>
@@ -1679,25 +1679,25 @@
         </is>
       </c>
       <c r="H29" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="I29" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J29" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>TF0064</t>
+          <t>TF0066</t>
         </is>
       </c>
       <c r="B30" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-13:47:52</t>
+15:47:51</t>
         </is>
       </c>
       <c r="C30" s="6" t="inlineStr">
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E30" s="6" t="inlineStr">
         <is>
-          <t>Dian</t>
+          <t>Hanny</t>
         </is>
       </c>
       <c r="F30" s="8" t="n">
@@ -1720,29 +1720,29 @@
       </c>
       <c r="G30" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H30" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
       <c r="I30" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J30" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>TF0065</t>
+          <t>TF0067</t>
         </is>
       </c>
       <c r="B31" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-14:38:42</t>
+17:08:48</t>
         </is>
       </c>
       <c r="C31" s="6" t="inlineStr">
@@ -1752,12 +1752,12 @@
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>08</t>
         </is>
       </c>
       <c r="E31" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F31" s="8" t="n">
@@ -1781,13 +1781,13 @@
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>TF0066</t>
+          <t>TF0068</t>
         </is>
       </c>
       <c r="B32" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-15:47:51</t>
+17:09:35</t>
         </is>
       </c>
       <c r="C32" s="6" t="inlineStr">
@@ -1797,12 +1797,12 @@
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>09</t>
         </is>
       </c>
       <c r="E32" s="6" t="inlineStr">
         <is>
-          <t>Hanny</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F32" s="8" t="n">
@@ -1810,29 +1810,29 @@
       </c>
       <c r="G32" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H32" s="8" t="n">
-        <v>495000</v>
+        <v>550000</v>
       </c>
       <c r="I32" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J32" s="8" t="n">
-        <v>495000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
         <is>
-          <t>TF0067</t>
+          <t>TF0069</t>
         </is>
       </c>
       <c r="B33" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-17:08:48</t>
+18:45:53</t>
         </is>
       </c>
       <c r="C33" s="6" t="inlineStr">
@@ -1842,16 +1842,16 @@
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>01</t>
         </is>
       </c>
       <c r="E33" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>andin</t>
         </is>
       </c>
       <c r="F33" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="G33" s="6" t="inlineStr">
         <is>
@@ -1859,25 +1859,25 @@
         </is>
       </c>
       <c r="H33" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="I33" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J33" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
         <is>
-          <t>TF0068</t>
+          <t>TF0070</t>
         </is>
       </c>
       <c r="B34" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-17:09:35</t>
+19:10:34</t>
         </is>
       </c>
       <c r="C34" s="6" t="inlineStr">
@@ -1887,16 +1887,16 @@
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>02</t>
         </is>
       </c>
       <c r="E34" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F34" s="8" t="n">
-        <v>550000</v>
+        <v>800000</v>
       </c>
       <c r="G34" s="6" t="inlineStr">
         <is>
@@ -1904,25 +1904,25 @@
         </is>
       </c>
       <c r="H34" s="8" t="n">
-        <v>550000</v>
+        <v>800000</v>
       </c>
       <c r="I34" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J34" s="8" t="n">
-        <v>550000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
         <is>
-          <t>TF0069</t>
+          <t>TF0071</t>
         </is>
       </c>
       <c r="B35" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-18:45:53</t>
+19:11:13</t>
         </is>
       </c>
       <c r="C35" s="6" t="inlineStr">
@@ -1932,16 +1932,16 @@
       </c>
       <c r="D35" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E35" s="6" t="inlineStr">
         <is>
-          <t>andin</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F35" s="8" t="n">
-        <v>550000</v>
+        <v>800000</v>
       </c>
       <c r="G35" s="6" t="inlineStr">
         <is>
@@ -1949,25 +1949,25 @@
         </is>
       </c>
       <c r="H35" s="8" t="n">
-        <v>550000</v>
+        <v>800000</v>
       </c>
       <c r="I35" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J35" s="8" t="n">
-        <v>550000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
         <is>
-          <t>TF0070</t>
+          <t>TF0072</t>
         </is>
       </c>
       <c r="B36" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-19:10:34</t>
+21:20:09</t>
         </is>
       </c>
       <c r="C36" s="6" t="inlineStr">
@@ -1977,16 +1977,16 @@
       </c>
       <c r="D36" s="6" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="E36" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Nadia</t>
         </is>
       </c>
       <c r="F36" s="8" t="n">
-        <v>800000</v>
+        <v>550000</v>
       </c>
       <c r="G36" s="6" t="inlineStr">
         <is>
@@ -1994,25 +1994,25 @@
         </is>
       </c>
       <c r="H36" s="8" t="n">
-        <v>800000</v>
+        <v>550000</v>
       </c>
       <c r="I36" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J36" s="8" t="n">
-        <v>800000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
         <is>
-          <t>TF0071</t>
+          <t>TF0073</t>
         </is>
       </c>
       <c r="B37" s="7" t="inlineStr">
         <is>
           <t>21-06-2025
-19:11:13</t>
+21:20:43</t>
         </is>
       </c>
       <c r="C37" s="6" t="inlineStr">
@@ -2022,16 +2022,16 @@
       </c>
       <c r="D37" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>05</t>
         </is>
       </c>
       <c r="E37" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Qila</t>
         </is>
       </c>
       <c r="F37" s="8" t="n">
-        <v>800000</v>
+        <v>550000</v>
       </c>
       <c r="G37" s="6" t="inlineStr">
         <is>
@@ -2039,25 +2039,25 @@
         </is>
       </c>
       <c r="H37" s="8" t="n">
-        <v>800000</v>
+        <v>550000</v>
       </c>
       <c r="I37" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J37" s="8" t="n">
-        <v>800000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
         <is>
-          <t>TF0072</t>
+          <t>TF0074</t>
         </is>
       </c>
       <c r="B38" s="7" t="inlineStr">
         <is>
-          <t>21-06-2025
-21:20:09</t>
+          <t>22-06-2025
+10:21:34</t>
         </is>
       </c>
       <c r="C38" s="6" t="inlineStr">
@@ -2067,12 +2067,12 @@
       </c>
       <c r="D38" s="6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>01</t>
         </is>
       </c>
       <c r="E38" s="6" t="inlineStr">
         <is>
-          <t>Nadia</t>
+          <t>Febby</t>
         </is>
       </c>
       <c r="F38" s="8" t="n">
@@ -2096,13 +2096,13 @@
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
         <is>
-          <t>TF0073</t>
+          <t>TF0075</t>
         </is>
       </c>
       <c r="B39" s="7" t="inlineStr">
         <is>
-          <t>21-06-2025
-21:20:43</t>
+          <t>22-06-2025
+11:11:14</t>
         </is>
       </c>
       <c r="C39" s="6" t="inlineStr">
@@ -2112,42 +2112,42 @@
       </c>
       <c r="D39" s="6" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E39" s="6" t="inlineStr">
         <is>
-          <t>Qila</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F39" s="8" t="n">
-        <v>550000</v>
+        <v>825000</v>
       </c>
       <c r="G39" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H39" s="8" t="n">
-        <v>550000</v>
+        <v>742500</v>
       </c>
       <c r="I39" s="8" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="J39" s="8" t="n">
-        <v>550000</v>
+        <v>743000</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="inlineStr">
         <is>
-          <t>TF0074</t>
+          <t>TF0076</t>
         </is>
       </c>
       <c r="B40" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-10:21:34</t>
+13:25:08</t>
         </is>
       </c>
       <c r="C40" s="6" t="inlineStr">
@@ -2157,12 +2157,12 @@
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>02</t>
         </is>
       </c>
       <c r="E40" s="6" t="inlineStr">
         <is>
-          <t>Febby</t>
+          <t>Dian</t>
         </is>
       </c>
       <c r="F40" s="8" t="n">
@@ -2186,13 +2186,13 @@
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
         <is>
-          <t>TF0075</t>
+          <t>TF0078</t>
         </is>
       </c>
       <c r="B41" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-11:11:14</t>
+13:47:09</t>
         </is>
       </c>
       <c r="C41" s="6" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E41" s="6" t="inlineStr">
@@ -2211,7 +2211,7 @@
         </is>
       </c>
       <c r="F41" s="8" t="n">
-        <v>825000</v>
+        <v>550000</v>
       </c>
       <c r="G41" s="6" t="inlineStr">
         <is>
@@ -2219,25 +2219,25 @@
         </is>
       </c>
       <c r="H41" s="8" t="n">
-        <v>742500</v>
+        <v>495000</v>
       </c>
       <c r="I41" s="8" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J41" s="8" t="n">
-        <v>743000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>TF0076</t>
+          <t>TF0079</t>
         </is>
       </c>
       <c r="B42" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-13:25:08</t>
+13:47:51</t>
         </is>
       </c>
       <c r="C42" s="6" t="inlineStr">
@@ -2247,12 +2247,12 @@
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="E42" s="6" t="inlineStr">
         <is>
-          <t>Dian</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F42" s="8" t="n">
@@ -2260,29 +2260,29 @@
       </c>
       <c r="G42" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H42" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
       <c r="I42" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J42" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
         <is>
-          <t>TF0078</t>
+          <t>TF0080</t>
         </is>
       </c>
       <c r="B43" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-13:47:09</t>
+13:51:08</t>
         </is>
       </c>
       <c r="C43" s="6" t="inlineStr">
@@ -2292,12 +2292,12 @@
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>05</t>
         </is>
       </c>
       <c r="E43" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Nadia</t>
         </is>
       </c>
       <c r="F43" s="8" t="n">
@@ -2305,29 +2305,29 @@
       </c>
       <c r="G43" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H43" s="8" t="n">
-        <v>495000</v>
+        <v>550000</v>
       </c>
       <c r="I43" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="8" t="n">
-        <v>495000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
         <is>
-          <t>TF0079</t>
+          <t>TF0082</t>
         </is>
       </c>
       <c r="B44" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-13:47:51</t>
+14:23:00</t>
         </is>
       </c>
       <c r="C44" s="6" t="inlineStr">
@@ -2337,42 +2337,42 @@
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E44" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Hanny</t>
         </is>
       </c>
       <c r="F44" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
       <c r="G44" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H44" s="8" t="n">
-        <v>495000</v>
+        <v>700000</v>
       </c>
       <c r="I44" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="8" t="n">
-        <v>495000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
         <is>
-          <t>TF0080</t>
+          <t>TF0083</t>
         </is>
       </c>
       <c r="B45" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-13:51:08</t>
+15:59:01</t>
         </is>
       </c>
       <c r="C45" s="6" t="inlineStr">
@@ -2382,42 +2382,42 @@
       </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E45" s="6" t="inlineStr">
         <is>
-          <t>Nadia</t>
+          <t>andin</t>
         </is>
       </c>
       <c r="F45" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="G45" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H45" s="8" t="n">
-        <v>550000</v>
+        <v>585000</v>
       </c>
       <c r="I45" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J45" s="8" t="n">
-        <v>550000</v>
+        <v>585000</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
         <is>
-          <t>TF0082</t>
+          <t>TF0084</t>
         </is>
       </c>
       <c r="B46" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-14:23:00</t>
+16:08:12</t>
         </is>
       </c>
       <c r="C46" s="6" t="inlineStr">
@@ -2427,16 +2427,16 @@
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>08</t>
         </is>
       </c>
       <c r="E46" s="6" t="inlineStr">
         <is>
-          <t>Hanny</t>
+          <t>Qila</t>
         </is>
       </c>
       <c r="F46" s="8" t="n">
-        <v>700000</v>
+        <v>550000</v>
       </c>
       <c r="G46" s="6" t="inlineStr">
         <is>
@@ -2444,25 +2444,25 @@
         </is>
       </c>
       <c r="H46" s="8" t="n">
-        <v>700000</v>
+        <v>550000</v>
       </c>
       <c r="I46" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="8" t="n">
-        <v>700000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
         <is>
-          <t>TF0083</t>
+          <t>TF0085</t>
         </is>
       </c>
       <c r="B47" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-15:59:01</t>
+16:16:56</t>
         </is>
       </c>
       <c r="C47" s="6" t="inlineStr">
@@ -2472,42 +2472,42 @@
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>09</t>
         </is>
       </c>
       <c r="E47" s="6" t="inlineStr">
         <is>
-          <t>andin</t>
+          <t>Dian</t>
         </is>
       </c>
       <c r="F47" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="G47" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H47" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
       <c r="I47" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J47" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
         <is>
-          <t>TF0084</t>
+          <t>TF0086</t>
         </is>
       </c>
       <c r="B48" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-16:08:12</t>
+16:24:08</t>
         </is>
       </c>
       <c r="C48" s="6" t="inlineStr">
@@ -2517,12 +2517,12 @@
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>01</t>
         </is>
       </c>
       <c r="E48" s="6" t="inlineStr">
         <is>
-          <t>Qila</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F48" s="8" t="n">
@@ -2546,13 +2546,13 @@
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
         <is>
-          <t>TF0085</t>
+          <t>TF0087</t>
         </is>
       </c>
       <c r="B49" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-16:16:56</t>
+16:36:17</t>
         </is>
       </c>
       <c r="C49" s="6" t="inlineStr">
@@ -2562,12 +2562,12 @@
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>02</t>
         </is>
       </c>
       <c r="E49" s="6" t="inlineStr">
         <is>
-          <t>Dian</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F49" s="8" t="n">
@@ -2591,13 +2591,13 @@
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
         <is>
-          <t>TF0086</t>
+          <t>TF0088</t>
         </is>
       </c>
       <c r="B50" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-16:24:08</t>
+18:59:10</t>
         </is>
       </c>
       <c r="C50" s="6" t="inlineStr">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E50" s="6" t="inlineStr">
@@ -2620,29 +2620,29 @@
       </c>
       <c r="G50" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H50" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
       <c r="I50" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J50" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="6" t="inlineStr">
         <is>
-          <t>TF0087</t>
+          <t>TF0089</t>
         </is>
       </c>
       <c r="B51" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-16:36:17</t>
+18:59:40</t>
         </is>
       </c>
       <c r="C51" s="6" t="inlineStr">
@@ -2652,7 +2652,7 @@
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="E51" s="6" t="inlineStr">
@@ -2661,33 +2661,33 @@
         </is>
       </c>
       <c r="F51" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="G51" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H51" s="8" t="n">
-        <v>550000</v>
+        <v>585000</v>
       </c>
       <c r="I51" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J51" s="8" t="n">
-        <v>550000</v>
+        <v>585000</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
         <is>
-          <t>TF0088</t>
+          <t>TF0090</t>
         </is>
       </c>
       <c r="B52" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-18:59:10</t>
+20:03:58</t>
         </is>
       </c>
       <c r="C52" s="6" t="inlineStr">
@@ -2697,16 +2697,16 @@
       </c>
       <c r="D52" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>05</t>
         </is>
       </c>
       <c r="E52" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Nadia</t>
         </is>
       </c>
       <c r="F52" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
       <c r="G52" s="6" t="inlineStr">
         <is>
@@ -2714,25 +2714,25 @@
         </is>
       </c>
       <c r="H52" s="8" t="n">
-        <v>495000</v>
+        <v>630000</v>
       </c>
       <c r="I52" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J52" s="8" t="n">
-        <v>495000</v>
+        <v>630000</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="inlineStr">
         <is>
-          <t>TF0089</t>
+          <t>TF0091</t>
         </is>
       </c>
       <c r="B53" s="7" t="inlineStr">
         <is>
           <t>22-06-2025
-18:59:40</t>
+21:23:18</t>
         </is>
       </c>
       <c r="C53" s="6" t="inlineStr">
@@ -2742,42 +2742,42 @@
       </c>
       <c r="D53" s="6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E53" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Febby</t>
         </is>
       </c>
       <c r="F53" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="G53" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H53" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
       <c r="I53" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J53" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="6" t="inlineStr">
         <is>
-          <t>TF0090</t>
+          <t>TF0094</t>
         </is>
       </c>
       <c r="B54" s="7" t="inlineStr">
         <is>
-          <t>22-06-2025
-20:03:58</t>
+          <t>24-06-2025
+12:08:11</t>
         </is>
       </c>
       <c r="C54" s="6" t="inlineStr">
@@ -2787,16 +2787,16 @@
       </c>
       <c r="D54" s="6" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>01</t>
         </is>
       </c>
       <c r="E54" s="6" t="inlineStr">
         <is>
-          <t>Nadia</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F54" s="8" t="n">
-        <v>700000</v>
+        <v>650000</v>
       </c>
       <c r="G54" s="6" t="inlineStr">
         <is>
@@ -2804,25 +2804,25 @@
         </is>
       </c>
       <c r="H54" s="8" t="n">
-        <v>630000</v>
+        <v>585000</v>
       </c>
       <c r="I54" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J54" s="8" t="n">
-        <v>630000</v>
+        <v>585000</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="6" t="inlineStr">
         <is>
-          <t>TF0091</t>
+          <t>TF0095</t>
         </is>
       </c>
       <c r="B55" s="7" t="inlineStr">
         <is>
-          <t>22-06-2025
-21:23:18</t>
+          <t>24-06-2025
+12:25:48</t>
         </is>
       </c>
       <c r="C55" s="6" t="inlineStr">
@@ -2832,12 +2832,12 @@
       </c>
       <c r="D55" s="6" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>02</t>
         </is>
       </c>
       <c r="E55" s="6" t="inlineStr">
         <is>
-          <t>Febby</t>
+          <t>Qila</t>
         </is>
       </c>
       <c r="F55" s="8" t="n">
@@ -2861,58 +2861,58 @@
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
         <is>
-          <t>TF0092</t>
+          <t>TF0096</t>
         </is>
       </c>
       <c r="B56" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-11:37:43</t>
+12:37:54</t>
         </is>
       </c>
       <c r="C56" s="6" t="inlineStr">
         <is>
-          <t>fnb</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="D56" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E56" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F56" s="8" t="n">
-        <v>35000</v>
+        <v>550000</v>
       </c>
       <c r="G56" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H56" s="8" t="n">
-        <v>35000</v>
+        <v>495000</v>
       </c>
       <c r="I56" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J56" s="8" t="n">
-        <v>35000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
         <is>
-          <t>TF0093</t>
+          <t>TF0097</t>
         </is>
       </c>
       <c r="B57" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-11:42:11</t>
+14:34:28</t>
         </is>
       </c>
       <c r="C57" s="6" t="inlineStr">
@@ -2922,12 +2922,12 @@
       </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E57" s="6" t="inlineStr">
         <is>
-          <t>andin</t>
+          <t>Hanny</t>
         </is>
       </c>
       <c r="F57" s="8" t="n">
@@ -2951,13 +2951,13 @@
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
         <is>
-          <t>TF0094</t>
+          <t>TF0098</t>
         </is>
       </c>
       <c r="B58" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-12:08:11</t>
+14:57:35</t>
         </is>
       </c>
       <c r="C58" s="6" t="inlineStr">
@@ -2967,42 +2967,42 @@
       </c>
       <c r="D58" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>04</t>
         </is>
       </c>
       <c r="E58" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Sherly</t>
         </is>
       </c>
       <c r="F58" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="G58" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H58" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
       <c r="I58" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J58" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="6" t="inlineStr">
         <is>
-          <t>TF0095</t>
+          <t>TF0099</t>
         </is>
       </c>
       <c r="B59" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-12:25:48</t>
+14:59:39</t>
         </is>
       </c>
       <c r="C59" s="6" t="inlineStr">
@@ -3012,12 +3012,12 @@
       </c>
       <c r="D59" s="6" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>05</t>
         </is>
       </c>
       <c r="E59" s="6" t="inlineStr">
         <is>
-          <t>Qila</t>
+          <t>Nadia</t>
         </is>
       </c>
       <c r="F59" s="8" t="n">
@@ -3041,13 +3041,13 @@
     <row r="60">
       <c r="A60" s="6" t="inlineStr">
         <is>
-          <t>TF0096</t>
+          <t>TF0100</t>
         </is>
       </c>
       <c r="B60" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-12:37:54</t>
+15:00:05</t>
         </is>
       </c>
       <c r="C60" s="6" t="inlineStr">
@@ -3057,12 +3057,12 @@
       </c>
       <c r="D60" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E60" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Febby</t>
         </is>
       </c>
       <c r="F60" s="8" t="n">
@@ -3070,29 +3070,29 @@
       </c>
       <c r="G60" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H60" s="8" t="n">
-        <v>495000</v>
+        <v>550000</v>
       </c>
       <c r="I60" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J60" s="8" t="n">
-        <v>495000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="6" t="inlineStr">
         <is>
-          <t>TF0097</t>
+          <t>TF0101</t>
         </is>
       </c>
       <c r="B61" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-14:34:28</t>
+16:29:06</t>
         </is>
       </c>
       <c r="C61" s="6" t="inlineStr">
@@ -3102,42 +3102,42 @@
       </c>
       <c r="D61" s="6" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>08</t>
         </is>
       </c>
       <c r="E61" s="6" t="inlineStr">
         <is>
-          <t>Hanny</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F61" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="G61" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H61" s="8" t="n">
-        <v>550000</v>
+        <v>585000</v>
       </c>
       <c r="I61" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J61" s="8" t="n">
-        <v>550000</v>
+        <v>585000</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="6" t="inlineStr">
         <is>
-          <t>TF0098</t>
+          <t>TF0102</t>
         </is>
       </c>
       <c r="B62" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-14:57:35</t>
+16:40:08</t>
         </is>
       </c>
       <c r="C62" s="6" t="inlineStr">
@@ -3147,7 +3147,7 @@
       </c>
       <c r="D62" s="6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>09</t>
         </is>
       </c>
       <c r="E62" s="6" t="inlineStr">
@@ -3156,7 +3156,7 @@
         </is>
       </c>
       <c r="F62" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="G62" s="6" t="inlineStr">
         <is>
@@ -3164,25 +3164,25 @@
         </is>
       </c>
       <c r="H62" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="I62" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J62" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="6" t="inlineStr">
         <is>
-          <t>TF0099</t>
+          <t>TF0103</t>
         </is>
       </c>
       <c r="B63" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-14:59:39</t>
+17:14:09</t>
         </is>
       </c>
       <c r="C63" s="6" t="inlineStr">
@@ -3192,12 +3192,12 @@
       </c>
       <c r="D63" s="6" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>01</t>
         </is>
       </c>
       <c r="E63" s="6" t="inlineStr">
         <is>
-          <t>Nadia</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F63" s="8" t="n">
@@ -3205,29 +3205,29 @@
       </c>
       <c r="G63" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H63" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
       <c r="I63" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J63" s="8" t="n">
-        <v>550000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="6" t="inlineStr">
         <is>
-          <t>TF0100</t>
+          <t>TF0104</t>
         </is>
       </c>
       <c r="B64" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-15:00:05</t>
+17:33:57</t>
         </is>
       </c>
       <c r="C64" s="6" t="inlineStr">
@@ -3237,12 +3237,12 @@
       </c>
       <c r="D64" s="6" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>02</t>
         </is>
       </c>
       <c r="E64" s="6" t="inlineStr">
         <is>
-          <t>Febby</t>
+          <t>andin</t>
         </is>
       </c>
       <c r="F64" s="8" t="n">
@@ -3266,13 +3266,13 @@
     <row r="65">
       <c r="A65" s="6" t="inlineStr">
         <is>
-          <t>TF0101</t>
+          <t>TF0105</t>
         </is>
       </c>
       <c r="B65" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-16:29:06</t>
+17:34:40</t>
         </is>
       </c>
       <c r="C65" s="6" t="inlineStr">
@@ -3282,12 +3282,12 @@
       </c>
       <c r="D65" s="6" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E65" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Febby</t>
         </is>
       </c>
       <c r="F65" s="8" t="n">
@@ -3311,13 +3311,13 @@
     <row r="66">
       <c r="A66" s="6" t="inlineStr">
         <is>
-          <t>TF0102</t>
+          <t>TF0106</t>
         </is>
       </c>
       <c r="B66" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-16:40:08</t>
+18:44:33</t>
         </is>
       </c>
       <c r="C66" s="6" t="inlineStr">
@@ -3327,7 +3327,7 @@
       </c>
       <c r="D66" s="6" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>04</t>
         </is>
       </c>
       <c r="E66" s="6" t="inlineStr">
@@ -3336,7 +3336,7 @@
         </is>
       </c>
       <c r="F66" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="G66" s="6" t="inlineStr">
         <is>
@@ -3344,70 +3344,70 @@
         </is>
       </c>
       <c r="H66" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="I66" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J66" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="6" t="inlineStr">
         <is>
-          <t>TF0103</t>
+          <t>TF0107</t>
         </is>
       </c>
       <c r="B67" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-17:14:09</t>
+19:22:30</t>
         </is>
       </c>
       <c r="C67" s="6" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>Fasilitas</t>
         </is>
       </c>
       <c r="D67" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E67" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F67" s="8" t="n">
-        <v>550000</v>
+        <v>200000</v>
       </c>
       <c r="G67" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H67" s="8" t="n">
-        <v>495000</v>
+        <v>200000</v>
       </c>
       <c r="I67" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J67" s="8" t="n">
-        <v>495000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="6" t="inlineStr">
         <is>
-          <t>TF0104</t>
+          <t>TF0108</t>
         </is>
       </c>
       <c r="B68" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-17:33:57</t>
+21:30:38</t>
         </is>
       </c>
       <c r="C68" s="6" t="inlineStr">
@@ -3417,16 +3417,16 @@
       </c>
       <c r="D68" s="6" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>05</t>
         </is>
       </c>
       <c r="E68" s="6" t="inlineStr">
         <is>
-          <t>andin</t>
+          <t>Ocha</t>
         </is>
       </c>
       <c r="F68" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="G68" s="6" t="inlineStr">
         <is>
@@ -3434,25 +3434,25 @@
         </is>
       </c>
       <c r="H68" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
       <c r="I68" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J68" s="8" t="n">
-        <v>550000</v>
+        <v>650000</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="6" t="inlineStr">
         <is>
-          <t>TF0105</t>
+          <t>TF0109</t>
         </is>
       </c>
       <c r="B69" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-17:34:40</t>
+21:31:06</t>
         </is>
       </c>
       <c r="C69" s="6" t="inlineStr">
@@ -3462,42 +3462,42 @@
       </c>
       <c r="D69" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E69" s="6" t="inlineStr">
         <is>
-          <t>Febby</t>
+          <t>Hanny</t>
         </is>
       </c>
       <c r="F69" s="8" t="n">
-        <v>650000</v>
+        <v>550000</v>
       </c>
       <c r="G69" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H69" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
       <c r="I69" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J69" s="8" t="n">
-        <v>585000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="6" t="inlineStr">
         <is>
-          <t>TF0106</t>
+          <t>TF0110</t>
         </is>
       </c>
       <c r="B70" s="7" t="inlineStr">
         <is>
           <t>24-06-2025
-18:44:33</t>
+21:31:37</t>
         </is>
       </c>
       <c r="C70" s="6" t="inlineStr">
@@ -3507,12 +3507,12 @@
       </c>
       <c r="D70" s="6" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>07</t>
         </is>
       </c>
       <c r="E70" s="6" t="inlineStr">
         <is>
-          <t>Sherly</t>
+          <t>Qila</t>
         </is>
       </c>
       <c r="F70" s="8" t="n">
@@ -3536,32 +3536,32 @@
     <row r="71">
       <c r="A71" s="6" t="inlineStr">
         <is>
-          <t>TF0107</t>
+          <t>TF0111</t>
         </is>
       </c>
       <c r="B71" s="7" t="inlineStr">
         <is>
-          <t>24-06-2025
-19:22:30</t>
+          <t>25-06-2025
+10:26:02</t>
         </is>
       </c>
       <c r="C71" s="6" t="inlineStr">
         <is>
-          <t>Fasilitas</t>
+          <t>massage</t>
         </is>
       </c>
       <c r="D71" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>01</t>
         </is>
       </c>
       <c r="E71" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F71" s="8" t="n">
-        <v>200000</v>
+        <v>700000</v>
       </c>
       <c r="G71" s="6" t="inlineStr">
         <is>
@@ -3569,25 +3569,25 @@
         </is>
       </c>
       <c r="H71" s="8" t="n">
-        <v>200000</v>
+        <v>700000</v>
       </c>
       <c r="I71" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J71" s="8" t="n">
-        <v>200000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="6" t="inlineStr">
         <is>
-          <t>TF0108</t>
+          <t>TF0112</t>
         </is>
       </c>
       <c r="B72" s="7" t="inlineStr">
         <is>
-          <t>24-06-2025
-21:30:38</t>
+          <t>25-06-2025
+10:56:56</t>
         </is>
       </c>
       <c r="C72" s="6" t="inlineStr">
@@ -3597,7 +3597,7 @@
       </c>
       <c r="D72" s="6" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>02</t>
         </is>
       </c>
       <c r="E72" s="6" t="inlineStr">
@@ -3610,29 +3610,29 @@
       </c>
       <c r="G72" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H72" s="8" t="n">
-        <v>650000</v>
+        <v>585000</v>
       </c>
       <c r="I72" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J72" s="8" t="n">
-        <v>650000</v>
+        <v>585000</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="6" t="inlineStr">
         <is>
-          <t>TF0109</t>
+          <t>TF0113</t>
         </is>
       </c>
       <c r="B73" s="7" t="inlineStr">
         <is>
-          <t>24-06-2025
-21:31:06</t>
+          <t>25-06-2025
+12:46:25</t>
         </is>
       </c>
       <c r="C73" s="6" t="inlineStr">
@@ -3642,16 +3642,16 @@
       </c>
       <c r="D73" s="6" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>03</t>
         </is>
       </c>
       <c r="E73" s="6" t="inlineStr">
         <is>
-          <t>Hanny</t>
+          <t>Dian</t>
         </is>
       </c>
       <c r="F73" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
       <c r="G73" s="6" t="inlineStr">
         <is>
@@ -3659,25 +3659,25 @@
         </is>
       </c>
       <c r="H73" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
       <c r="I73" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J73" s="8" t="n">
-        <v>550000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="6" t="inlineStr">
         <is>
-          <t>TF0110</t>
+          <t>TF0114</t>
         </is>
       </c>
       <c r="B74" s="7" t="inlineStr">
         <is>
-          <t>24-06-2025
-21:31:37</t>
+          <t>25-06-2025
+13:07:26</t>
         </is>
       </c>
       <c r="C74" s="6" t="inlineStr">
@@ -3687,42 +3687,42 @@
       </c>
       <c r="D74" s="6" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="E74" s="6" t="inlineStr">
         <is>
-          <t>Qila</t>
+          <t>Lia</t>
         </is>
       </c>
       <c r="F74" s="8" t="n">
-        <v>550000</v>
+        <v>825000</v>
       </c>
       <c r="G74" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H74" s="8" t="n">
-        <v>550000</v>
+        <v>742500</v>
       </c>
       <c r="I74" s="8" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="J74" s="8" t="n">
-        <v>550000</v>
+        <v>743000</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="6" t="inlineStr">
         <is>
-          <t>TF0111</t>
+          <t>TF0115</t>
         </is>
       </c>
       <c r="B75" s="7" t="inlineStr">
         <is>
           <t>25-06-2025
-10:26:02</t>
+14:42:08</t>
         </is>
       </c>
       <c r="C75" s="6" t="inlineStr">
@@ -3732,42 +3732,42 @@
       </c>
       <c r="D75" s="6" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>KTV01</t>
         </is>
       </c>
       <c r="E75" s="6" t="inlineStr">
         <is>
-          <t>Lia</t>
+          <t>Nadia</t>
         </is>
       </c>
       <c r="F75" s="8" t="n">
-        <v>700000</v>
+        <v>2000000</v>
       </c>
       <c r="G75" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="H75" s="8" t="n">
-        <v>700000</v>
+        <v>1800000</v>
       </c>
       <c r="I75" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J75" s="8" t="n">
-        <v>700000</v>
+        <v>1800000</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="6" t="inlineStr">
         <is>
-          <t>TF0112</t>
+          <t>TF0116</t>
         </is>
       </c>
       <c r="B76" s="7" t="inlineStr">
         <is>
-          <t>25-06-2025
-10:56:56</t>
+          <t>28-06-2025
+18:00:01</t>
         </is>
       </c>
       <c r="C76" s="6" t="inlineStr">
@@ -3782,56 +3782,56 @@
       </c>
       <c r="E76" s="6" t="inlineStr">
         <is>
-          <t>Ocha</t>
+          <t>Sherly</t>
         </is>
       </c>
       <c r="F76" s="8" t="n">
-        <v>650000</v>
+        <v>700000</v>
       </c>
       <c r="G76" s="6" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H76" s="8" t="n">
-        <v>585000</v>
+        <v>800000</v>
       </c>
       <c r="I76" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J76" s="8" t="n">
-        <v>585000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="6" t="inlineStr">
         <is>
-          <t>TF0113</t>
+          <t>TF0117</t>
         </is>
       </c>
       <c r="B77" s="7" t="inlineStr">
         <is>
-          <t>25-06-2025
-12:46:25</t>
+          <t>29-06-2025
+00:46:46</t>
         </is>
       </c>
       <c r="C77" s="6" t="inlineStr">
         <is>
-          <t>massage</t>
+          <t>fnb</t>
         </is>
       </c>
       <c r="D77" s="6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E77" s="6" t="inlineStr">
         <is>
-          <t>Dian</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F77" s="8" t="n">
-        <v>700000</v>
+        <v>50000</v>
       </c>
       <c r="G77" s="6" t="inlineStr">
         <is>
@@ -3839,391 +3839,76 @@
         </is>
       </c>
       <c r="H77" s="8" t="n">
-        <v>700000</v>
+        <v>50000</v>
       </c>
       <c r="I77" s="8" t="n">
         <v>0</v>
       </c>
       <c r="J77" s="8" t="n">
-        <v>700000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="6" t="inlineStr">
         <is>
-          <t>TF0114</t>
+          <t>TF0118</t>
         </is>
       </c>
       <c r="B78" s="7" t="inlineStr">
-        <is>
-          <t>25-06-2025
-13:07:26</t>
-        </is>
-      </c>
-      <c r="C78" s="6" t="inlineStr">
-        <is>
-          <t>massage</t>
-        </is>
-      </c>
-      <c r="D78" s="6" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="E78" s="6" t="inlineStr">
-        <is>
-          <t>Lia</t>
-        </is>
-      </c>
-      <c r="F78" s="8" t="n">
-        <v>825000</v>
-      </c>
-      <c r="G78" s="6" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="H78" s="8" t="n">
-        <v>742500</v>
-      </c>
-      <c r="I78" s="8" t="n">
-        <v>500</v>
-      </c>
-      <c r="J78" s="8" t="n">
-        <v>743000</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="6" t="inlineStr">
-        <is>
-          <t>TF0115</t>
-        </is>
-      </c>
-      <c r="B79" s="7" t="inlineStr">
-        <is>
-          <t>25-06-2025
-14:42:08</t>
-        </is>
-      </c>
-      <c r="C79" s="6" t="inlineStr">
-        <is>
-          <t>massage</t>
-        </is>
-      </c>
-      <c r="D79" s="6" t="inlineStr">
-        <is>
-          <t>KTV01</t>
-        </is>
-      </c>
-      <c r="E79" s="6" t="inlineStr">
-        <is>
-          <t>Nadia</t>
-        </is>
-      </c>
-      <c r="F79" s="8" t="n">
-        <v>2000000</v>
-      </c>
-      <c r="G79" s="6" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="H79" s="8" t="n">
-        <v>1800000</v>
-      </c>
-      <c r="I79" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" s="8" t="n">
-        <v>1800000</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="6" t="inlineStr">
-        <is>
-          <t>TF0116</t>
-        </is>
-      </c>
-      <c r="B80" s="7" t="inlineStr">
-        <is>
-          <t>28-06-2025
-18:00:01</t>
-        </is>
-      </c>
-      <c r="C80" s="6" t="inlineStr">
-        <is>
-          <t>massage</t>
-        </is>
-      </c>
-      <c r="D80" s="6" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="E80" s="6" t="inlineStr">
-        <is>
-          <t>Sherly</t>
-        </is>
-      </c>
-      <c r="F80" s="8" t="n">
-        <v>700000</v>
-      </c>
-      <c r="G80" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H80" s="8" t="n">
-        <v>800000</v>
-      </c>
-      <c r="I80" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" s="8" t="n">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="6" t="inlineStr">
-        <is>
-          <t>TF0117</t>
-        </is>
-      </c>
-      <c r="B81" s="7" t="inlineStr">
-        <is>
-          <t>29-06-2025
-00:46:46</t>
-        </is>
-      </c>
-      <c r="C81" s="6" t="inlineStr">
-        <is>
-          <t>fnb</t>
-        </is>
-      </c>
-      <c r="D81" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E81" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F81" s="8" t="n">
-        <v>50000</v>
-      </c>
-      <c r="G81" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H81" s="8" t="n">
-        <v>50000</v>
-      </c>
-      <c r="I81" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J81" s="8" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="6" t="inlineStr">
-        <is>
-          <t>TF0118</t>
-        </is>
-      </c>
-      <c r="B82" s="7" t="inlineStr">
         <is>
           <t>30-06-2025
 15:44:25</t>
         </is>
       </c>
-      <c r="C82" s="6" t="inlineStr">
+      <c r="C78" s="6" t="inlineStr">
         <is>
           <t>fnb</t>
         </is>
       </c>
-      <c r="D82" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E82" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F82" s="8" t="n">
+      <c r="D78" s="6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E78" s="6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F78" s="8" t="n">
         <v>60000</v>
       </c>
-      <c r="G82" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H82" s="8" t="n">
+      <c r="G78" s="6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H78" s="8" t="n">
         <v>60000</v>
       </c>
-      <c r="I82" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J82" s="8" t="n">
+      <c r="I78" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="8" t="n">
         <v>60000</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="6" t="inlineStr">
-        <is>
-          <t>TF0119</t>
-        </is>
-      </c>
-      <c r="B83" s="7" t="inlineStr">
-        <is>
-          <t>30-06-2025
-16:19:06</t>
-        </is>
-      </c>
-      <c r="C83" s="6" t="inlineStr">
-        <is>
-          <t>massage</t>
-        </is>
-      </c>
-      <c r="D83" s="6" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="E83" s="6" t="inlineStr">
-        <is>
-          <t>andin</t>
-        </is>
-      </c>
-      <c r="F83" s="8" t="n">
-        <v>650000</v>
-      </c>
-      <c r="G83" s="6" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="H83" s="8" t="n">
-        <v>585000</v>
-      </c>
-      <c r="I83" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J83" s="8" t="n">
-        <v>585000</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="6" t="inlineStr">
-        <is>
-          <t>TF0120</t>
-        </is>
-      </c>
-      <c r="B84" s="7" t="inlineStr">
-        <is>
-          <t>30-06-2025
-16:47:40</t>
-        </is>
-      </c>
-      <c r="C84" s="6" t="inlineStr">
-        <is>
-          <t>massage</t>
-        </is>
-      </c>
-      <c r="D84" s="6" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="E84" s="6" t="inlineStr">
-        <is>
-          <t>andin</t>
-        </is>
-      </c>
-      <c r="F84" s="8" t="n">
-        <v>650000</v>
-      </c>
-      <c r="G84" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H84" s="8" t="n">
-        <v>650000</v>
-      </c>
-      <c r="I84" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J84" s="8" t="n">
-        <v>650000</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="6" t="inlineStr">
-        <is>
-          <t>TF0121</t>
-        </is>
-      </c>
-      <c r="B85" s="7" t="inlineStr">
-        <is>
-          <t>30-06-2025
-17:07:05</t>
-        </is>
-      </c>
-      <c r="C85" s="6" t="inlineStr">
-        <is>
-          <t>massage</t>
-        </is>
-      </c>
-      <c r="D85" s="6" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="E85" s="6" t="inlineStr">
-        <is>
-          <t>andin</t>
-        </is>
-      </c>
-      <c r="F85" s="8" t="n">
-        <v>650000</v>
-      </c>
-      <c r="G85" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H85" s="8" t="n">
-        <v>650000</v>
-      </c>
-      <c r="I85" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J85" s="8" t="n">
-        <v>650000</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="9" t="inlineStr">
+    <row r="80">
+      <c r="A80" s="9" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B87" s="9" t="inlineStr"/>
-      <c r="C87" s="9" t="inlineStr"/>
-      <c r="D87" s="9" t="inlineStr"/>
-      <c r="E87" s="9" t="inlineStr"/>
-      <c r="F87" s="9" t="inlineStr"/>
-      <c r="G87" s="9" t="inlineStr"/>
-      <c r="H87" s="9" t="inlineStr"/>
-      <c r="I87" s="9" t="inlineStr"/>
-      <c r="J87" s="10" t="n">
-        <v>52433500</v>
+      <c r="B80" s="9" t="inlineStr"/>
+      <c r="C80" s="9" t="inlineStr"/>
+      <c r="D80" s="9" t="inlineStr"/>
+      <c r="E80" s="9" t="inlineStr"/>
+      <c r="F80" s="9" t="inlineStr"/>
+      <c r="G80" s="9" t="inlineStr"/>
+      <c r="H80" s="9" t="inlineStr"/>
+      <c r="I80" s="9" t="inlineStr"/>
+      <c r="J80" s="10" t="n">
+        <v>48763500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>